<commit_message>
Test hierarchy mapping from YCL
</commit_message>
<xml_diff>
--- a/yti-taxgen-test-commons/src/main/resources/test_fixtures/ycl_source_config/codelist_comprehensive.xlsx
+++ b/yti-taxgen-test-commons/src/main/resources/test_fixtures/ycl_source_config/codelist_comprehensive.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="2960" windowWidth="28560" windowHeight="17380"/>
+    <workbookView xWindow="1760" yWindow="460" windowWidth="28800" windowHeight="17620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
     <sheet name="Codes_testfixture_codelist_comp" sheetId="2" r:id="rId2"/>
-    <sheet name="ExtensionSchemes_testfixture_co" sheetId="3" r:id="rId3"/>
+    <sheet name="Extensions_testfixture_codelist" sheetId="3" r:id="rId3"/>
+    <sheet name="Members_calc_hier_0" sheetId="4" r:id="rId4"/>
+    <sheet name="Members_def_hier_0" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="146">
   <si>
     <t>ID</t>
   </si>
@@ -40,7 +42,7 @@
     <t>ORGANIZATION</t>
   </si>
   <si>
-    <t>CLASSIFICATION</t>
+    <t>INFORMATIONDOMAIN</t>
   </si>
   <si>
     <t>LANGUAGECODE</t>
@@ -106,12 +108,18 @@
     <t>CODESSHEET</t>
   </si>
   <si>
-    <t>EXTENSIONSCHEMESSHEET</t>
+    <t>EXTENSIONSSHEET</t>
+  </si>
+  <si>
+    <t>5314a353-5ad4-4c81-8368-70495979e3c4</t>
   </si>
   <si>
     <t>testfixture_codelist_comprehensive</t>
   </si>
   <si>
+    <t>71837f4a-c503-4f3d-84dc-d645314528cf</t>
+  </si>
+  <si>
     <t>P9</t>
   </si>
   <si>
@@ -133,6 +141,9 @@
     <t>governancePolicy #noloc</t>
   </si>
   <si>
+    <t>code_1</t>
+  </si>
+  <si>
     <t>Test Fixture: Codelist Comprehensive #fi</t>
   </si>
   <si>
@@ -160,7 +171,7 @@
     <t>Codes_testfixture_codelist_comp</t>
   </si>
   <si>
-    <t>ExtensionSchemes_testfixture_co</t>
+    <t>Extensions_testfixture_codelist</t>
   </si>
   <si>
     <t>BROADER</t>
@@ -175,6 +186,9 @@
     <t>ORDER</t>
   </si>
   <si>
+    <t>eb81fdea-6c24-4e74-b159-f34a8d9dc476</t>
+  </si>
+  <si>
     <t>code_0</t>
   </si>
   <si>
@@ -199,10 +213,7 @@
     <t>Code 0 short name #noloc</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>code_1</t>
+    <t>2f13f036-21b9-4855-9457-a869fffd5bb8</t>
   </si>
   <si>
     <t>Code 1 #fi</t>
@@ -226,7 +237,7 @@
     <t>Code 1 short name #noloc</t>
   </si>
   <si>
-    <t>2</t>
+    <t>ea41b4e5-9551-428a-8e3f-45d85b9b326e</t>
   </si>
   <si>
     <t>code_2</t>
@@ -253,7 +264,58 @@
     <t>Code 2 short name #noloc</t>
   </si>
   <si>
-    <t>3</t>
+    <t>03e639f8-a4a3-49d1-8282-2b9a114e627f</t>
+  </si>
+  <si>
+    <t>code_3</t>
+  </si>
+  <si>
+    <t>Code 3 #fi</t>
+  </si>
+  <si>
+    <t>Code 3 #en</t>
+  </si>
+  <si>
+    <t>Code 3 definition #fi</t>
+  </si>
+  <si>
+    <t>Code 3 definition #en</t>
+  </si>
+  <si>
+    <t>Code 3 description #fi</t>
+  </si>
+  <si>
+    <t>Code 3 description #en</t>
+  </si>
+  <si>
+    <t>Code 3 short name #noloc</t>
+  </si>
+  <si>
+    <t>7d420e89-6239-4e98-bca5-c4d949cd119e</t>
+  </si>
+  <si>
+    <t>code_4</t>
+  </si>
+  <si>
+    <t>Code 4 #fi</t>
+  </si>
+  <si>
+    <t>Code 4 #en</t>
+  </si>
+  <si>
+    <t>Code 4 definition #fi</t>
+  </si>
+  <si>
+    <t>Code 4 definition #en</t>
+  </si>
+  <si>
+    <t>Code 4 description #fi</t>
+  </si>
+  <si>
+    <t>Code 4 description #en</t>
+  </si>
+  <si>
+    <t>Code 4 short name #noloc</t>
   </si>
   <si>
     <t>PROPERTYTYPE</t>
@@ -262,17 +324,169 @@
     <t>CODESCHEMES</t>
   </si>
   <si>
-    <t>EXTENSIONSSHEET</t>
+    <t>MEMBERSSHEET</t>
+  </si>
+  <si>
+    <t>66aa4c76-7763-4dfc-9c86-36c89e94db86</t>
+  </si>
+  <si>
+    <t>calc_hier_0</t>
+  </si>
+  <si>
+    <t>calculationHierarchy</t>
+  </si>
+  <si>
+    <t>Calculation hierachy 0 #fi</t>
+  </si>
+  <si>
+    <t>Calculation hierachy 0 #en</t>
+  </si>
+  <si>
+    <t>500543de-3906-4d17-a05e-676bf46488a4</t>
+  </si>
+  <si>
+    <t>def_hier_0</t>
+  </si>
+  <si>
+    <t>definitionHierarchy</t>
+  </si>
+  <si>
+    <t>Definition hierachy 0 #fi</t>
+  </si>
+  <si>
+    <t>Definition hierachy 0 #en</t>
+  </si>
+  <si>
+    <t>UNARYOPERATOR</t>
+  </si>
+  <si>
+    <t>COMPARISONOPERATOR</t>
+  </si>
+  <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>RELATION</t>
+  </si>
+  <si>
+    <t>067a9156-b657-4e5c-9bf6-35f7da4a4274</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Calculation member 1 #fi</t>
+  </si>
+  <si>
+    <t>Calculation member 1 #en</t>
+  </si>
+  <si>
+    <t>a8629f41-e3e0-4584-af8f-39868b3e2e59</t>
+  </si>
+  <si>
+    <t>Calculation member 2 #fi</t>
+  </si>
+  <si>
+    <t>Calculation member 2 #en</t>
+  </si>
+  <si>
+    <t>685b0e31-7801-458e-a65d-3d33d0e03e8d</t>
+  </si>
+  <si>
+    <t>Calculation member 3 #fi</t>
+  </si>
+  <si>
+    <t>Calculation member 3 #en</t>
+  </si>
+  <si>
+    <t>48f96daf-8ae6-45b6-9b1b-b2aec12fd5c2</t>
+  </si>
+  <si>
+    <t>Calculation member 4 #fi</t>
+  </si>
+  <si>
+    <t>Calculation member 4 #en</t>
+  </si>
+  <si>
+    <t>d9f3ab1f-fc31-466f-8085-058673122a86</t>
+  </si>
+  <si>
+    <t>Calculation member 0 #fi</t>
+  </si>
+  <si>
+    <t>Calculation member 0 #en</t>
+  </si>
+  <si>
+    <t>bafd19a7-4bf0-434a-ad2d-a891f26016d9</t>
+  </si>
+  <si>
+    <t>Definition member 0 #fi</t>
+  </si>
+  <si>
+    <t>Definition member 0 #en</t>
+  </si>
+  <si>
+    <t>50c530d9-06ea-4680-99c4-bd150a8586a7</t>
+  </si>
+  <si>
+    <t>Definition member 1 #fi</t>
+  </si>
+  <si>
+    <t>Definition member 1 #en</t>
+  </si>
+  <si>
+    <t>2f4a5e8b-e0d0-4640-91e3-12bbadff5487</t>
+  </si>
+  <si>
+    <t>Definition member 2 #fi</t>
+  </si>
+  <si>
+    <t>Definition member 2 #en</t>
+  </si>
+  <si>
+    <t>c0382929-1a40-40dd-8822-010cc35f04e5</t>
+  </si>
+  <si>
+    <t>Definition member 3 #fi</t>
+  </si>
+  <si>
+    <t>Definition member 3 #en</t>
+  </si>
+  <si>
+    <t>42fb1f4e-d1ec-4eea-af72-15eadd0fed49</t>
+  </si>
+  <si>
+    <t>Definition member 4 #fi</t>
+  </si>
+  <si>
+    <t>Definition member 4 #en</t>
+  </si>
+  <si>
+    <t>Members_calc_hier_0</t>
+  </si>
+  <si>
+    <t>Members_def_hier_0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -295,13 +509,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -579,11 +798,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="13" max="13" width="32.33203125" customWidth="1"/>
+    <col min="14" max="14" width="33" customWidth="1"/>
+    <col min="25" max="25" width="29.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -666,88 +891,93 @@
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L2" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="M2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="N2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="O2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="P2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="Q2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="R2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="S2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="T2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="U2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="V2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Y2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="Z2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="38.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -757,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -781,16 +1011,16 @@
         <v>17</v>
       </c>
       <c r="K1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L1" t="s">
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="N1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O1" t="s">
         <v>20</v>
@@ -806,144 +1036,253 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="K2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" t="s">
-        <v>56</v>
+        <v>33</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="J3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>56</v>
-      </c>
-      <c r="N3" t="s">
-        <v>65</v>
+        <v>33</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
       </c>
       <c r="O3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="L4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" t="s">
-        <v>74</v>
+        <v>33</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
       </c>
       <c r="O4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P4" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6" t="s">
+        <v>94</v>
+      </c>
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -953,27 +1292,369 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45.6640625" customWidth="1"/>
+    <col min="6" max="7" width="30.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="F1" t="s">
         <v>20</v>
@@ -988,7 +1669,137 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>77</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>